<commit_message>
Connect Database & Model
</commit_message>
<xml_diff>
--- a/Backend/src/configs/data.xlsx
+++ b/Backend/src/configs/data.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>lesson</t>
   </si>
 </sst>
 </file>
@@ -379,17 +379,17 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -397,7 +397,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -405,7 +405,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -413,7 +413,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -421,7 +421,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -429,7 +429,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>